<commit_message>
adding finished payload schematic layout
</commit_message>
<xml_diff>
--- a/payload2020_bom.xlsx
+++ b/payload2020_bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adampaul/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adampaul/Documents/Payload-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A40E0C3-DD61-E348-B20A-C3E36E014EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B852D3A9-1452-564F-BC08-9EFDEDE51A34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20300" xr2:uid="{698FD68D-CA3A-5844-BC42-7BE57830F418}"/>
+    <workbookView xWindow="14200" yWindow="2180" windowWidth="25720" windowHeight="20300" xr2:uid="{698FD68D-CA3A-5844-BC42-7BE57830F418}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t>Ref numbers</t>
   </si>
@@ -57,17 +57,397 @@
     <t>Base Board</t>
   </si>
   <si>
-    <t>D1, D2, D3</t>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>22pF Capacitor</t>
+  </si>
+  <si>
+    <t>311-1062-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/CC0603JRNPO9BN220/311-1062-1-ND/302972</t>
+  </si>
+  <si>
+    <t>0.1uF Capacitor</t>
+  </si>
+  <si>
+    <t>1276-1258-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/samsung-electro-mechanics/CL10F104ZO8NNNC/1276-1258-1-ND/3889344</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/CC0603KRX7R9BB561/302813</t>
+  </si>
+  <si>
+    <t>560pF Capacitor</t>
+  </si>
+  <si>
+    <t>311-1079-2-ND</t>
+  </si>
+  <si>
+    <t>490-14372-2-ND</t>
+  </si>
+  <si>
+    <t>10uF Capacitor</t>
+  </si>
+  <si>
+    <t>C4, C5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/murata-electronics/GRM188R61A106KE69J/6606001</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/CC0603KRX7R9BB332/302816</t>
+  </si>
+  <si>
+    <t>3.3nF Capacitor</t>
+  </si>
+  <si>
+    <t>311-1082-2-ND</t>
+  </si>
+  <si>
+    <t>22uF Capacitor</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>47uF Capacitor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/murata-electronics/GRM188R60J226MEA0D/4280542</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/murata-electronics/GRM188C80E476ME05D/5877407</t>
+  </si>
+  <si>
+    <t>490-13244-2-ND</t>
+  </si>
+  <si>
+    <t>490-7611-2-ND</t>
+  </si>
+  <si>
+    <t>Orange Debug LED</t>
+  </si>
+  <si>
+    <t>1080-1586-2-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/everlight-electronics-co-ltd/19-217-S2C-AM2N2VY-3T/8535280</t>
+  </si>
+  <si>
+    <t>JP1-15</t>
+  </si>
+  <si>
+    <t>2 pin jumper male</t>
+  </si>
+  <si>
+    <t>2 pin jumper female</t>
+  </si>
+  <si>
+    <t>952-2262-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/harwin-inc/M20-9990246/3728226</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sullins-connector-solutions/QPC02SXGN-RC/2618262</t>
+  </si>
+  <si>
+    <t>S9337-ND</t>
+  </si>
+  <si>
+    <t>J1, J4, J6</t>
+  </si>
+  <si>
+    <t>Harwin 2x3 connector male</t>
+  </si>
+  <si>
+    <t>Harwin 2x3 connector female</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>Harwin 2x4 connector male</t>
+  </si>
+  <si>
+    <t>Harwin 2x4 connector female</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/harwin-inc/M80-5000642/952-1000-5-ND/2263989</t>
+  </si>
+  <si>
+    <t>952-1000-5-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/harwin-inc/M80-5100842/952-2341-ND/3906370</t>
+  </si>
+  <si>
+    <t>952-2341-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/harwin-inc/M80-4180698/8251037</t>
+  </si>
+  <si>
+    <t>952-3779-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/harwin-inc/M80-4140898/8250990</t>
+  </si>
+  <si>
+    <t>952-3732-ND</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>2.2uH inductor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/eaton-electronics-division/MCL2012V1-2R2-R/10299846</t>
+  </si>
+  <si>
+    <t>283-MCL2012V1-2R2-RCT-ND</t>
+  </si>
+  <si>
+    <t>33uH inductor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/sumida-america-components-inc/CR54NP-330LC/956641</t>
+  </si>
+  <si>
+    <t>308-1535-2-ND</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>A1, A2</t>
+  </si>
+  <si>
+    <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t>C16, C17, C18</t>
+  </si>
+  <si>
+    <t>Power PMOS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/alpha-omega-semiconductor-inc/AO3415/785-1010-1-ND/1855952</t>
+  </si>
+  <si>
+    <t>785-1010-1-ND</t>
+  </si>
+  <si>
+    <t>R3-5, R7, R10, R12-R24, R31-R33</t>
+  </si>
+  <si>
+    <t>10k pullup resistor</t>
+  </si>
+  <si>
+    <t>311-10KGRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/RC0603JR-0710KL/311-10KGRCT-ND/729647</t>
+  </si>
+  <si>
+    <t>100k Pullup</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>RR08P100KDCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/susumu/RR0816P-104-D/RR08P100KDCT-ND/432772</t>
+  </si>
+  <si>
+    <t>4.7k Resistor</t>
+  </si>
+  <si>
+    <t>100 ohm resistor</t>
+  </si>
+  <si>
+    <t>R25, R28</t>
+  </si>
+  <si>
+    <t>R26, R27, R29, R30</t>
+  </si>
+  <si>
+    <t>311-4.70KHRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/RC0603FR-074K7L/311-4.70KHRCT-ND/730159</t>
+  </si>
+  <si>
+    <t>311-100HRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/yageo/RC0603FR-07100RL/311-100HRCT-ND/729835</t>
+  </si>
+  <si>
+    <t>D1, D5, D6</t>
+  </si>
+  <si>
+    <t>Q1, Q4, Q5</t>
+  </si>
+  <si>
+    <t>R1, R8, R9</t>
+  </si>
+  <si>
+    <t>120 ohm resistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/te-connectivity-passive-product/CRGCQ0603F120R/A129677CT-ND/8577509</t>
+  </si>
+  <si>
+    <t>A129677CT-ND</t>
+  </si>
+  <si>
+    <t>digikey.ca/product-detail/en/te-connectivity-alcoswitch-switches/1825910-6/450-1650-ND/1632536</t>
+  </si>
+  <si>
+    <t>Pushbutton Switch</t>
+  </si>
+  <si>
+    <t>450-1650-ND</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>CAN Controller</t>
+  </si>
+  <si>
+    <t>U1, U5</t>
+  </si>
+  <si>
+    <t>CAN Transceiver</t>
+  </si>
+  <si>
+    <t>U4, U8</t>
+  </si>
+  <si>
+    <t>U2, U3</t>
+  </si>
+  <si>
+    <t>Adafruit SD Breakout</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>5v Switching Regulator</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>12v boost regulator</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>I2C level shifter</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>Altimeter</t>
+  </si>
+  <si>
+    <t>Y1, Y2</t>
+  </si>
+  <si>
+    <t>Oscillator</t>
+  </si>
+  <si>
+    <t>MCP2515-E/SO-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/microchip-technology/MCP2515-E-SO/593677</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/microchip-technology/MCP2562-E-SN/4079967?s=N4IgTCBcDaILIGEAKYCsA2MBaAogegGUA5EAXQF8g</t>
+  </si>
+  <si>
+    <t>MCP2562-E/SN-ND</t>
+  </si>
+  <si>
+    <t>296-39448-2-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/TPS62143RGTR/2833437</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/linear-technology-analog-devices/LT1109ACS8-12-PBF/LT1109ACS8-12-PBF-ND/890895</t>
+  </si>
+  <si>
+    <t>LT1109ACS8-12#PBF-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/TCA9517DGKR/296-35972-1-ND/4135104</t>
+  </si>
+  <si>
+    <t>296-35972-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-measurement-specialties/MS560702BA03-50/223-1198-1-ND/4700921</t>
+  </si>
+  <si>
+    <t>223-1198-1-ND</t>
+  </si>
+  <si>
+    <t>C6, C3, C13</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/molex/1040310811/WM6357CT-ND/2804769</t>
+  </si>
+  <si>
+    <t>SD Card Slot</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/LD1117S33TR/497-1242-1-ND/586242</t>
+  </si>
+  <si>
+    <t>3.3v linear regulator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/texas-instruments/CD74HC4050M96/296-14529-1-ND/555596</t>
+  </si>
+  <si>
+    <t>Logic shifter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,13 +470,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,16 +792,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9790478-AFF6-5548-B461-BFC082497DF6}">
-  <dimension ref="A2:H4"/>
+  <dimension ref="A2:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
@@ -458,8 +841,661 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0.15</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0.31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0.15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0.4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0.76</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>0.6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>0.17</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>0.15</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>12.35</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>8.34</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>6.95</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0.34</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1.36</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>0.15</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0.15</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>0.15</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>0.15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>0.15</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>0.15</v>
+      </c>
+      <c r="G27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>3.18</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>1.38</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>3.18</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1.01</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>3.78</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>132</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{CA84E48C-B9A2-7C4A-A4B5-49E70067FCF1}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{EAACE498-76ED-2240-9F14-BC03268CFD4E}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{202C90D7-D5DC-4641-AA63-BC4C048216B5}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{4946F454-2101-534F-9E14-6EDC241E93D5}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{56FB4254-1390-1C4B-8F51-89966EF4208D}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{2F618648-AFA2-CF4E-8E08-BDCAB3826C9E}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{1FB65E80-741D-CA47-8EBC-405412E41ED8}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{AE4CD88D-C40C-5C41-86FD-74D7E7875FD8}"/>
+    <hyperlink ref="G12" r:id="rId9" xr:uid="{83D20C4B-CB03-CD46-B9D0-FFA1C9B81EDD}"/>
+    <hyperlink ref="G13" r:id="rId10" xr:uid="{CEB3E3A0-59E2-5F47-A003-4CF98C849CB8}"/>
+    <hyperlink ref="G14" r:id="rId11" xr:uid="{84183DC6-9665-BB49-B59A-31CC607BC285}"/>
+    <hyperlink ref="G16" r:id="rId12" xr:uid="{17AC049A-6224-EB4D-9D0A-C0E9668B53CB}"/>
+    <hyperlink ref="G15" r:id="rId13" xr:uid="{4658BDA4-9580-8B43-AFF7-682FF1CD76B5}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{44747501-EF2F-7342-9DFA-3391170937F6}"/>
+    <hyperlink ref="G18" r:id="rId15" xr:uid="{65CD9784-1869-A749-A1A5-8B3394B58FF2}"/>
+    <hyperlink ref="G19" r:id="rId16" xr:uid="{C26116ED-D27D-8D40-8C47-7E4E5D1FB07C}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{B049D3A9-7F1A-AB42-A968-3D1CE3B279F4}"/>
+    <hyperlink ref="G22" r:id="rId18" xr:uid="{439FCC4A-3C9C-0A43-8447-0A836F9FA755}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{2FBF9D73-CC0E-1D41-8FC7-4675ED562105}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{EC219639-D3B5-C548-8491-E62854440DAF}"/>
+    <hyperlink ref="G25" r:id="rId21" xr:uid="{9A13B3DB-F555-A844-9824-3B02C1594642}"/>
+    <hyperlink ref="G26" r:id="rId22" xr:uid="{378D9BF2-B062-9F4A-B813-48EF71447431}"/>
+    <hyperlink ref="G28" r:id="rId23" xr:uid="{56C8C56F-A30D-2C42-B74B-2A09F726C710}"/>
+    <hyperlink ref="G29" r:id="rId24" xr:uid="{41DA5166-2603-664B-A25E-FCFC14CB87E0}"/>
+    <hyperlink ref="G31" r:id="rId25" xr:uid="{45F0F9D6-A9EC-4047-8ACA-17825235BB7A}"/>
+    <hyperlink ref="G32" r:id="rId26" xr:uid="{61F3542F-AF9C-5D43-952F-00DCC14110A4}"/>
+    <hyperlink ref="G33" r:id="rId27" xr:uid="{CE75FA50-5608-FA4D-B083-9A0AE9036F32}"/>
+    <hyperlink ref="G34" r:id="rId28" xr:uid="{A73C2A8C-D537-BA4A-A033-AC0270902F97}"/>
+    <hyperlink ref="G36" r:id="rId29" xr:uid="{41EFBE9A-84E4-474E-A4C0-5E152CC1A5DD}"/>
+    <hyperlink ref="G37" r:id="rId30" xr:uid="{F0C0C617-2E45-3148-9A03-E63B0659CEBC}"/>
+    <hyperlink ref="G38" r:id="rId31" xr:uid="{2B4E8C49-D24A-D844-8969-2475CF37C91C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated schematic based on aarons PR comments
</commit_message>
<xml_diff>
--- a/payload2020_bom.xlsx
+++ b/payload2020_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adampaul/Documents/Payload-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B852D3A9-1452-564F-BC08-9EFDEDE51A34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F919E0AE-3294-6448-8772-8878F92DCF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14200" yWindow="2180" windowWidth="25720" windowHeight="20300" xr2:uid="{698FD68D-CA3A-5844-BC42-7BE57830F418}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>Ref numbers</t>
   </si>
@@ -300,9 +300,6 @@
     <t>D1, D5, D6</t>
   </si>
   <si>
-    <t>Q1, Q4, Q5</t>
-  </si>
-  <si>
     <t>R1, R8, R9</t>
   </si>
   <si>
@@ -430,6 +427,21 @@
   </si>
   <si>
     <t>Logic shifter</t>
+  </si>
+  <si>
+    <t>Q1,  Q5</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>NMOS power</t>
+  </si>
+  <si>
+    <t>785-1460-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/alpha-omega-semiconductor-inc/AO3434A/785-1460-1-ND/3603468</t>
   </si>
 </sst>
 </file>
@@ -792,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9790478-AFF6-5548-B461-BFC082497DF6}">
-  <dimension ref="A2:H38"/>
+  <dimension ref="A2:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,7 +911,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1161,7 +1173,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
         <v>69</v>
@@ -1261,13 +1273,13 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
         <v>90</v>
       </c>
-      <c r="C26" t="s">
-        <v>91</v>
-      </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -1276,18 +1288,18 @@
         <v>0.15</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
         <v>95</v>
-      </c>
-      <c r="D27" t="s">
-        <v>96</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1296,18 +1308,18 @@
         <v>0.15</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1316,18 +1328,18 @@
         <v>3.18</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -1336,26 +1348,26 @@
         <v>1.38</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s">
         <v>102</v>
-      </c>
-      <c r="C30" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" t="s">
         <v>104</v>
       </c>
-      <c r="C31" t="s">
-        <v>105</v>
-      </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1364,18 +1376,18 @@
         <v>3.18</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
         <v>106</v>
       </c>
-      <c r="C32" t="s">
-        <v>107</v>
-      </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1384,18 +1396,18 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" t="s">
         <v>108</v>
       </c>
-      <c r="C33" t="s">
-        <v>109</v>
-      </c>
       <c r="D33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1404,18 +1416,18 @@
         <v>1.01</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
         <v>110</v>
       </c>
-      <c r="C34" t="s">
-        <v>111</v>
-      </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1424,15 +1436,15 @@
         <v>3.78</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" t="s">
         <v>112</v>
-      </c>
-      <c r="C35" t="s">
-        <v>113</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -1440,26 +1452,46 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0.6</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1495,6 +1527,7 @@
     <hyperlink ref="G36" r:id="rId29" xr:uid="{41EFBE9A-84E4-474E-A4C0-5E152CC1A5DD}"/>
     <hyperlink ref="G37" r:id="rId30" xr:uid="{F0C0C617-2E45-3148-9A03-E63B0659CEBC}"/>
     <hyperlink ref="G38" r:id="rId31" xr:uid="{2B4E8C49-D24A-D844-8969-2475CF37C91C}"/>
+    <hyperlink ref="G39" r:id="rId32" xr:uid="{B5E76BF1-7A82-1642-A803-58CA83F496E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>